<commit_message>
Added bootstrapping version for XGBoost
</commit_message>
<xml_diff>
--- a/Datasets/model_mape_hsc.xlsx
+++ b/Datasets/model_mape_hsc.xlsx
@@ -460,13 +460,13 @@
         <v>15.8356310742549</v>
       </c>
       <c r="B2" t="n">
-        <v>22.65019692829418</v>
+        <v>18.5523435399542</v>
       </c>
       <c r="C2" t="n">
-        <v>19.28163756635473</v>
+        <v>17.55742921144385</v>
       </c>
       <c r="D2" t="n">
-        <v>13.24284629626024</v>
+        <v>11.96228717994154</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>0.6059371906405118</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3706194701432692</v>
+        <v>0.3649964739644579</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4008032985598141</v>
+        <v>0.2624334960621995</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2946163817214444</v>
+        <v>0.2870668474823946</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>0.6802978596155157</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9761681163870162</v>
+        <v>0.3485797187544966</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9786478700095429</v>
+        <v>0.6427828021627909</v>
       </c>
       <c r="D4" t="n">
-        <v>0.285466055152561</v>
+        <v>0.2556116864232861</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>0.3458615333434216</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5427606586581193</v>
+        <v>0.2851189159817535</v>
       </c>
       <c r="C5" t="n">
-        <v>4.033032001248118</v>
+        <v>0.4085519896680884</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2714834709038582</v>
+        <v>0.2528149115790507</v>
       </c>
     </row>
     <row r="6">
@@ -516,27 +516,27 @@
         <v>4.334124189940244</v>
       </c>
       <c r="B6" t="n">
-        <v>5.126475365673104</v>
+        <v>4.921550602529484</v>
       </c>
       <c r="C6" t="n">
-        <v>4.497267966126322</v>
+        <v>4.136497483818174</v>
       </c>
       <c r="D6" t="n">
-        <v>4.181816142841215</v>
+        <v>4.574839854008596</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.5201984925609868</v>
+        <v>0.5019609516481496</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4860620588511519</v>
+        <v>0.4312174909554408</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4337861204492878</v>
+        <v>0.4839749065006404</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2774419414444567</v>
+        <v>0.2327944710257013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>